<commit_message>
Add General Table to accept any sheet
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="students" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -35,12 +35,6 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Munerah Alzaidan</t>
-  </si>
-  <si>
-    <t>University</t>
-  </si>
-  <si>
     <t>King Saud University</t>
   </si>
   <si>
@@ -57,6 +51,12 @@
   </si>
   <si>
     <t>student four name</t>
+  </si>
+  <si>
+    <t>Munerah Alzaidan2</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -389,7 +389,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -397,10 +397,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>441204576</v>
@@ -408,10 +408,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>583392224</v>
@@ -419,10 +419,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>343534534</v>
@@ -430,10 +430,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>358373736</v>
@@ -441,10 +441,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>309538715</v>
@@ -452,10 +452,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>260703694</v>
@@ -463,10 +463,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>211868673</v>
@@ -474,10 +474,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>163033652</v>
@@ -485,10 +485,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>114198631</v>
@@ -496,10 +496,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>653634610</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>165284589</v>
@@ -518,10 +518,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>323046432</v>
@@ -529,10 +529,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>814141453</v>

</xml_diff>